<commit_message>
Added new forms and added new data structure problem that arrange all zero to left side of an given array
</commit_message>
<xml_diff>
--- a/WindowsFormsApplication3/NoteBook/Book1.xlsx
+++ b/WindowsFormsApplication3/NoteBook/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guthanga\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Study\WindowsFormsApplication3\NoteBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Add</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t xml:space="preserve">List&lt;Int&gt; que </t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>I+1</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -148,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -158,6 +167,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -921,9 +931,102 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E33">
         <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B35" s="5">
+        <v>0</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5">
+        <v>2</v>
+      </c>
+      <c r="E35" s="5">
+        <v>3</v>
+      </c>
+      <c r="F35" s="5">
+        <v>4</v>
+      </c>
+      <c r="G35" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="G40" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="E41" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added graph breadth first, depth first travel, first occurance of character data structure puzzle
</commit_message>
<xml_diff>
--- a/WindowsFormsApplication3/NoteBook/Book1.xlsx
+++ b/WindowsFormsApplication3/NoteBook/Book1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Add</t>
   </si>
@@ -89,15 +89,6 @@
     <t>Shift right(&gt;&gt;)</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Call</t>
-  </si>
-  <si>
-    <t>Put</t>
-  </si>
-  <si>
     <t xml:space="preserve">List&lt;Int&gt; que </t>
   </si>
   <si>
@@ -108,6 +99,30 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>Arrange all 0 to left in the given array</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -448,16 +463,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.08984375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -931,12 +946,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E33">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B35" s="5">
         <v>0</v>
       </c>
@@ -956,7 +976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>1</v>
       </c>
@@ -976,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>1</v>
       </c>
@@ -996,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>1</v>
       </c>
@@ -1016,17 +1036,76 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G40" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="E41" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
         <v>26</v>
+      </c>
+      <c r="C44" t="str">
+        <f>"-&gt;B,C"</f>
+        <v>-&gt;B,C</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" t="str">
+        <f>"-&gt;A,C,D"</f>
+        <v>-&gt;A,C,D</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" t="str">
+        <f>"-&gt;B,D"</f>
+        <v>-&gt;B,D</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" t="str">
+        <f>"-&gt;B,C"</f>
+        <v>-&gt;B,C</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="str">
+        <f>"-&gt;F"</f>
+        <v>-&gt;F</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" t="str">
+        <f>"-&gt;E"</f>
+        <v>-&gt;E</v>
       </c>
     </row>
   </sheetData>
@@ -1040,7 +1119,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1127,7 +1206,7 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1137,110 +1216,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1">
-        <f>A2</f>
-        <v>-59.120000000000118</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1">
-        <f>F2</f>
-        <v>486.13000000000005</v>
-      </c>
-      <c r="K1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1">
-        <f>K2</f>
-        <v>-99.69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <f>SUM(C3:C4)-D3</f>
-        <v>-59.120000000000118</v>
-      </c>
-      <c r="F2">
-        <f>SUM(H3:H4)-SUM(I3:I4)</f>
-        <v>486.13000000000005</v>
-      </c>
-      <c r="K2">
-        <f>SUM(M3:M4)-N3</f>
-        <v>-99.69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3">
-        <v>1155</v>
-      </c>
-      <c r="C3">
-        <v>920.04</v>
-      </c>
-      <c r="D3">
-        <v>1719.2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3">
-        <v>1775.5</v>
-      </c>
-      <c r="H3">
-        <v>376.04</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3">
-        <v>92.5</v>
-      </c>
-      <c r="M3">
-        <v>390.42</v>
-      </c>
-      <c r="N3">
-        <v>490.11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>1152.5</v>
-      </c>
-      <c r="C4">
-        <v>740.04</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4">
-        <v>1772.5</v>
-      </c>
-      <c r="H4">
-        <v>400.04</v>
-      </c>
-      <c r="I4">
-        <v>289.95</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>